<commit_message>
updated check_directionarl_overlap, added link to post_treatment recurrence
</commit_message>
<xml_diff>
--- a/Volumes.xlsx
+++ b/Volumes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmanderson\Desktop\Local_Recurrence_Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Modular_Projects\Liver_Disease_Ablation_Segmentation\Local_Recurrence_Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ablation</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>% Reduced</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -354,7 +357,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +533,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
       <c r="C15" s="1">
         <f>AVERAGE(C2:C14)</f>
         <v>37.49363581211616</v>

</xml_diff>